<commit_message>
test: update tests for import wizard and geocoding changes
- Expand E2E import wizard tests
- Add geocoding provider rate limiter tests
- Update job tests for new geocoding behavior
- Add event creation helpers tests
</commit_message>
<xml_diff>
--- a/apps/web/tests/fixtures/multi-sheet.xlsx
+++ b/apps/web/tests/fixtures/multi-sheet.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <workbookPr codeName="ThisWorkbook"/>
   <sheets>
-    <sheet name="Events" sheetId="1" r:id="rId1"/>
-    <sheet name="Locations" sheetId="2" r:id="rId2"/>
-    <sheet name="Categories" sheetId="3" r:id="rId3"/>
+    <sheet name="Tech Events" sheetId="1" r:id="rId1"/>
+    <sheet name="Art Exhibitions" sheetId="2" r:id="rId2"/>
+    <sheet name="Sports Events" sheetId="3" r:id="rId3"/>
   </sheets>
 </workbook>
 </file>
@@ -399,7 +399,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -409,44 +409,79 @@
         <v>title</v>
       </c>
       <c r="B1" t="str">
-        <v>date</v>
+        <v>event_date</v>
       </c>
       <c r="C1" t="str">
-        <v>category</v>
+        <v>venue</v>
+      </c>
+      <c r="D1" t="str">
+        <v>city</v>
+      </c>
+      <c r="E1" t="str">
+        <v>description</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Event 1</v>
+        <v>AI Summit 2024</v>
       </c>
       <c r="B2" t="str">
-        <v>2024-03-15</v>
+        <v>2024-06-15</v>
       </c>
       <c r="C2" t="str">
-        <v>technology</v>
+        <v>Tech Convention Center</v>
+      </c>
+      <c r="D2" t="str">
+        <v>San Francisco, CA</v>
+      </c>
+      <c r="E2" t="str">
+        <v>Annual conference on artificial intelligence trends</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Event 2</v>
+        <v>Web Dev Conference</v>
       </c>
       <c r="B3" t="str">
-        <v>2024-03-20</v>
+        <v>2024-06-20</v>
       </c>
       <c r="C3" t="str">
-        <v>arts</v>
+        <v>Digital Hub</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Austin, TX</v>
+      </c>
+      <c r="E3" t="str">
+        <v>Latest in web development technologies</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Startup Pitch Night</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2024-07-01</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Innovation Lab</v>
+      </c>
+      <c r="D4" t="str">
+        <v>Seattle, WA</v>
+      </c>
+      <c r="E4" t="str">
+        <v>Early-stage startups present to investors</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E4"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -456,75 +491,163 @@
         <v>name</v>
       </c>
       <c r="B1" t="str">
-        <v>address</v>
+        <v>date</v>
       </c>
       <c r="C1" t="str">
-        <v>capacity</v>
+        <v>location</v>
+      </c>
+      <c r="D1" t="str">
+        <v>details</v>
+      </c>
+      <c r="E1" t="str">
+        <v>category</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>Convention Center</v>
+        <v>Modern Masters Exhibition</v>
       </c>
       <c r="B2" t="str">
-        <v>123 Main St</v>
+        <v>2024-07-10</v>
       </c>
       <c r="C2" t="str">
-        <v>1000</v>
+        <v>Metropolitan Art Museum, New York, NY</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Collection of 20th century masterpieces</v>
+      </c>
+      <c r="E2" t="str">
+        <v>painting</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>Art Gallery</v>
+        <v>Sculpture Garden Opening</v>
       </c>
       <c r="B3" t="str">
-        <v>456 Art Ave</v>
+        <v>2024-07-15</v>
       </c>
       <c r="C3" t="str">
-        <v>200</v>
+        <v>City Sculpture Park, Chicago, IL</v>
+      </c>
+      <c r="D3" t="str">
+        <v>Outdoor exhibition of contemporary sculptures</v>
+      </c>
+      <c r="E3" t="str">
+        <v>sculpture</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="str">
+        <v>Photography Retrospective</v>
+      </c>
+      <c r="B4" t="str">
+        <v>2024-08-01</v>
+      </c>
+      <c r="C4" t="str">
+        <v>Gallery of Fine Arts, Los Angeles, CA</v>
+      </c>
+      <c r="D4" t="str">
+        <v>50 years of documentary photography</v>
+      </c>
+      <c r="E4" t="str">
+        <v>photography</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Digital Art Fair</v>
+      </c>
+      <c r="B5" t="str">
+        <v>2024-08-10</v>
+      </c>
+      <c r="C5" t="str">
+        <v>Creative Center, Miami, FL</v>
+      </c>
+      <c r="D5" t="str">
+        <v>NFTs and digital installations</v>
+      </c>
+      <c r="E5" t="str">
+        <v>digital</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:C3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:E5"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetData>
     <row r="1">
       <c r="A1" t="str">
-        <v>category</v>
+        <v>event_name</v>
       </c>
       <c r="B1" t="str">
-        <v>description</v>
+        <v>start_date</v>
+      </c>
+      <c r="C1" t="str">
+        <v>address</v>
+      </c>
+      <c r="D1" t="str">
+        <v>lat</v>
+      </c>
+      <c r="E1" t="str">
+        <v>lng</v>
+      </c>
+      <c r="F1" t="str">
+        <v>notes</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="str">
-        <v>technology</v>
+        <v>City Marathon</v>
       </c>
       <c r="B2" t="str">
-        <v>Tech-related events</v>
+        <v>2024-09-01</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Central Park, New York, NY</v>
+      </c>
+      <c r="D2">
+        <v>40.7829</v>
+      </c>
+      <c r="E2">
+        <v>-73.9654</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Annual 26.2 mile race through the city</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="str">
-        <v>arts</v>
+        <v>Tennis Open</v>
       </c>
       <c r="B3" t="str">
-        <v>Arts and culture events</v>
+        <v>2024-09-15</v>
+      </c>
+      <c r="C3" t="str">
+        <v>National Tennis Center, Flushing, NY</v>
+      </c>
+      <c r="D3">
+        <v>40.7498</v>
+      </c>
+      <c r="E3">
+        <v>-73.8477</v>
+      </c>
+      <c r="F3" t="str">
+        <v>Professional tennis tournament</v>
       </c>
     </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:B3"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F3"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>